<commit_message>
modified:   devops/data/Classes.xlsx 	modified:   website/app.py 	modified:   website/static/js/script.js 	modified:   website/templates/index.html
</commit_message>
<xml_diff>
--- a/devops/data/Classes.xlsx
+++ b/devops/data/Classes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\AoE2\devops\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\AoE2\AoE2_Attack_Analyzer\AoE2_Attack_Analyzer\devops\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C17CAE-1776-47F4-A029-1DF8F0498447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD835F9-3A40-43FD-A4D9-AED968C0E935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="2980" windowWidth="23170" windowHeight="9860" xr2:uid="{CF94A639-838F-4DE8-90FE-EF32AB8D3BD9}"/>
+    <workbookView xWindow="26610" yWindow="2360" windowWidth="23170" windowHeight="9860" xr2:uid="{CF94A639-838F-4DE8-90FE-EF32AB8D3BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Infantry</t>
   </si>
   <si>
-    <t>Turtle Ships and Thirisadai</t>
-  </si>
-  <si>
     <t>Base Pierce</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>All Archers</t>
   </si>
   <si>
-    <t>High Pierce Armor Siege Units</t>
-  </si>
-  <si>
     <t>Trees</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Standard Buildings</t>
   </si>
   <si>
-    <t>Ships (except Fish ships)</t>
-  </si>
-  <si>
     <t>All Buildings</t>
   </si>
   <si>
@@ -146,10 +137,19 @@
     <t>Class Name</t>
   </si>
   <si>
-    <t>Stone Defense &amp; Harbors</t>
-  </si>
-  <si>
-    <t>Mounted Units (exc. Camels)</t>
+    <t>Turtle Ships &amp; Thirisadai</t>
+  </si>
+  <si>
+    <t>Stone Defense &amp; Harb.</t>
+  </si>
+  <si>
+    <t>High Pierce Arm. Siege</t>
+  </si>
+  <si>
+    <t>Mounted Units (excl. Camels)</t>
+  </si>
+  <si>
+    <t>Ships (excl. fishing ships)</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,10 +563,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -598,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -638,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -662,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -670,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -686,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -694,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -710,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -726,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -734,7 +734,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -742,7 +742,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -750,7 +750,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -758,7 +758,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -774,7 +774,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,7 +782,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -798,7 +798,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -814,7 +814,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,7 +838,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -854,7 +854,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -862,7 +862,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -870,7 +870,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -878,7 +878,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -886,7 +886,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>